<commit_message>
didn't have the labels right
</commit_message>
<xml_diff>
--- a/data/sizes/B_2023POGS_small_seed_daily/B_sizes_09132024.xlsx
+++ b/data/sizes/B_2023POGS_small_seed_daily/B_sizes_09132024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graceleuchtenberger/Library/Mobile Documents/com~apple~CloudDocs/Documents/project-gigas-conditioning-GL/data/sizes/B_2023POGS_small_seed_daily/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E00E80B9-BC3C-1B40-8FB6-DE33F47BF9D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3208A82A-D7B6-954E-905E-840B3978BDDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19000" windowHeight="21600" xr2:uid="{59562AC7-2699-D84F-A30D-CDAA438C0A0D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19000" windowHeight="19580" xr2:uid="{59562AC7-2699-D84F-A30D-CDAA438C0A0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -511,8 +511,8 @@
   <dimension ref="A1:XFC611"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A607" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G594" sqref="G594"/>
+      <pane ySplit="1" topLeftCell="A522" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D536" sqref="D536:D611"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -26569,7 +26569,7 @@
         <v>13</v>
       </c>
       <c r="D536" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E536" t="s">
         <v>15</v>
@@ -26610,7 +26610,7 @@
         <v>13</v>
       </c>
       <c r="D537" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E537" t="s">
         <v>15</v>
@@ -26651,7 +26651,7 @@
         <v>13</v>
       </c>
       <c r="D538" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E538" t="s">
         <v>15</v>
@@ -26692,7 +26692,7 @@
         <v>13</v>
       </c>
       <c r="D539" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E539" t="s">
         <v>15</v>
@@ -26733,7 +26733,7 @@
         <v>13</v>
       </c>
       <c r="D540" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E540" t="s">
         <v>15</v>
@@ -26774,7 +26774,7 @@
         <v>13</v>
       </c>
       <c r="D541" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E541" t="s">
         <v>15</v>
@@ -26815,7 +26815,7 @@
         <v>13</v>
       </c>
       <c r="D542" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E542" t="s">
         <v>15</v>
@@ -26856,7 +26856,7 @@
         <v>13</v>
       </c>
       <c r="D543" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E543" t="s">
         <v>15</v>
@@ -26897,7 +26897,7 @@
         <v>13</v>
       </c>
       <c r="D544" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E544" t="s">
         <v>15</v>
@@ -26938,7 +26938,7 @@
         <v>13</v>
       </c>
       <c r="D545" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E545" t="s">
         <v>15</v>
@@ -26979,7 +26979,7 @@
         <v>13</v>
       </c>
       <c r="D546" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E546" t="s">
         <v>15</v>
@@ -27020,7 +27020,7 @@
         <v>13</v>
       </c>
       <c r="D547" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E547" t="s">
         <v>15</v>
@@ -27061,7 +27061,7 @@
         <v>13</v>
       </c>
       <c r="D548" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E548" t="s">
         <v>15</v>
@@ -27102,7 +27102,7 @@
         <v>13</v>
       </c>
       <c r="D549" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E549" t="s">
         <v>15</v>
@@ -27143,7 +27143,7 @@
         <v>13</v>
       </c>
       <c r="D550" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E550" t="s">
         <v>15</v>
@@ -27184,7 +27184,7 @@
         <v>13</v>
       </c>
       <c r="D551" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E551" t="s">
         <v>15</v>
@@ -27225,7 +27225,7 @@
         <v>13</v>
       </c>
       <c r="D552" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E552" t="s">
         <v>15</v>
@@ -27266,7 +27266,7 @@
         <v>13</v>
       </c>
       <c r="D553" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E553" t="s">
         <v>15</v>
@@ -27307,7 +27307,7 @@
         <v>13</v>
       </c>
       <c r="D554" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E554" t="s">
         <v>15</v>
@@ -27348,7 +27348,7 @@
         <v>13</v>
       </c>
       <c r="D555" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E555" t="s">
         <v>15</v>
@@ -27389,7 +27389,7 @@
         <v>13</v>
       </c>
       <c r="D556" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E556" t="s">
         <v>15</v>
@@ -27430,7 +27430,7 @@
         <v>13</v>
       </c>
       <c r="D557" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E557" t="s">
         <v>15</v>
@@ -27471,7 +27471,7 @@
         <v>13</v>
       </c>
       <c r="D558" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E558" t="s">
         <v>15</v>
@@ -27512,7 +27512,7 @@
         <v>13</v>
       </c>
       <c r="D559" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E559" t="s">
         <v>15</v>
@@ -27553,7 +27553,7 @@
         <v>13</v>
       </c>
       <c r="D560" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E560" t="s">
         <v>15</v>
@@ -27594,7 +27594,7 @@
         <v>13</v>
       </c>
       <c r="D561" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E561" t="s">
         <v>15</v>
@@ -27635,7 +27635,7 @@
         <v>13</v>
       </c>
       <c r="D562" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E562" t="s">
         <v>15</v>
@@ -27676,7 +27676,7 @@
         <v>13</v>
       </c>
       <c r="D563" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E563" t="s">
         <v>15</v>
@@ -27717,7 +27717,7 @@
         <v>13</v>
       </c>
       <c r="D564" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E564" t="s">
         <v>15</v>
@@ -27758,7 +27758,7 @@
         <v>13</v>
       </c>
       <c r="D565" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E565" t="s">
         <v>15</v>
@@ -27799,7 +27799,7 @@
         <v>13</v>
       </c>
       <c r="D566" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E566" t="s">
         <v>15</v>
@@ -27840,7 +27840,7 @@
         <v>13</v>
       </c>
       <c r="D567" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E567" t="s">
         <v>15</v>
@@ -27881,7 +27881,7 @@
         <v>13</v>
       </c>
       <c r="D568" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E568" t="s">
         <v>15</v>
@@ -27922,7 +27922,7 @@
         <v>13</v>
       </c>
       <c r="D569" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E569" t="s">
         <v>15</v>
@@ -27963,7 +27963,7 @@
         <v>13</v>
       </c>
       <c r="D570" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E570" t="s">
         <v>15</v>
@@ -28004,7 +28004,7 @@
         <v>13</v>
       </c>
       <c r="D571" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E571" t="s">
         <v>15</v>
@@ -28045,7 +28045,7 @@
         <v>13</v>
       </c>
       <c r="D572" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E572" t="s">
         <v>15</v>
@@ -28086,7 +28086,7 @@
         <v>13</v>
       </c>
       <c r="D573" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E573" t="s">
         <v>15</v>
@@ -28127,7 +28127,7 @@
         <v>13</v>
       </c>
       <c r="D574" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E574" t="s">
         <v>15</v>
@@ -28168,7 +28168,7 @@
         <v>13</v>
       </c>
       <c r="D575" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E575" t="s">
         <v>15</v>
@@ -28209,7 +28209,7 @@
         <v>13</v>
       </c>
       <c r="D576" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E576" t="s">
         <v>15</v>
@@ -28250,7 +28250,7 @@
         <v>13</v>
       </c>
       <c r="D577" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E577" t="s">
         <v>15</v>
@@ -28291,7 +28291,7 @@
         <v>13</v>
       </c>
       <c r="D578" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E578" t="s">
         <v>15</v>
@@ -28332,7 +28332,7 @@
         <v>13</v>
       </c>
       <c r="D579" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E579" t="s">
         <v>15</v>
@@ -28373,7 +28373,7 @@
         <v>13</v>
       </c>
       <c r="D580" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E580" t="s">
         <v>15</v>
@@ -28414,7 +28414,7 @@
         <v>13</v>
       </c>
       <c r="D581" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E581" t="s">
         <v>15</v>
@@ -28455,7 +28455,7 @@
         <v>13</v>
       </c>
       <c r="D582" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E582" t="s">
         <v>15</v>
@@ -28496,7 +28496,7 @@
         <v>13</v>
       </c>
       <c r="D583" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E583" t="s">
         <v>15</v>
@@ -28537,7 +28537,7 @@
         <v>13</v>
       </c>
       <c r="D584" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E584" t="s">
         <v>15</v>
@@ -28578,7 +28578,7 @@
         <v>13</v>
       </c>
       <c r="D585" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E585" t="s">
         <v>15</v>
@@ -28619,7 +28619,7 @@
         <v>13</v>
       </c>
       <c r="D586" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E586" t="s">
         <v>15</v>
@@ -28660,7 +28660,7 @@
         <v>13</v>
       </c>
       <c r="D587" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E587" t="s">
         <v>15</v>
@@ -28701,7 +28701,7 @@
         <v>13</v>
       </c>
       <c r="D588" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E588" t="s">
         <v>15</v>
@@ -28742,7 +28742,7 @@
         <v>13</v>
       </c>
       <c r="D589" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E589" t="s">
         <v>15</v>
@@ -28783,7 +28783,7 @@
         <v>13</v>
       </c>
       <c r="D590" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E590" t="s">
         <v>15</v>
@@ -28824,7 +28824,7 @@
         <v>13</v>
       </c>
       <c r="D591" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E591" t="s">
         <v>15</v>
@@ -28865,7 +28865,7 @@
         <v>13</v>
       </c>
       <c r="D592" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E592" t="s">
         <v>15</v>
@@ -28906,7 +28906,7 @@
         <v>13</v>
       </c>
       <c r="D593" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E593" t="s">
         <v>15</v>
@@ -28947,7 +28947,7 @@
         <v>13</v>
       </c>
       <c r="D594" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E594" t="s">
         <v>15</v>
@@ -28988,7 +28988,7 @@
         <v>13</v>
       </c>
       <c r="D595" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E595" t="s">
         <v>15</v>
@@ -29029,7 +29029,7 @@
         <v>13</v>
       </c>
       <c r="D596" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E596" t="s">
         <v>15</v>
@@ -29070,7 +29070,7 @@
         <v>13</v>
       </c>
       <c r="D597" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E597" t="s">
         <v>15</v>
@@ -29111,7 +29111,7 @@
         <v>13</v>
       </c>
       <c r="D598" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E598" t="s">
         <v>15</v>
@@ -29152,7 +29152,7 @@
         <v>13</v>
       </c>
       <c r="D599" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E599" t="s">
         <v>15</v>
@@ -29193,7 +29193,7 @@
         <v>13</v>
       </c>
       <c r="D600" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E600" t="s">
         <v>15</v>
@@ -29234,7 +29234,7 @@
         <v>13</v>
       </c>
       <c r="D601" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E601" t="s">
         <v>15</v>
@@ -29275,7 +29275,7 @@
         <v>13</v>
       </c>
       <c r="D602" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E602" t="s">
         <v>15</v>
@@ -29316,7 +29316,7 @@
         <v>13</v>
       </c>
       <c r="D603" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E603" t="s">
         <v>15</v>
@@ -29357,7 +29357,7 @@
         <v>13</v>
       </c>
       <c r="D604" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E604" t="s">
         <v>15</v>
@@ -29398,7 +29398,7 @@
         <v>13</v>
       </c>
       <c r="D605" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E605" t="s">
         <v>15</v>
@@ -29439,7 +29439,7 @@
         <v>13</v>
       </c>
       <c r="D606" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E606" t="s">
         <v>15</v>
@@ -29480,7 +29480,7 @@
         <v>13</v>
       </c>
       <c r="D607" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E607" t="s">
         <v>15</v>
@@ -29521,7 +29521,7 @@
         <v>13</v>
       </c>
       <c r="D608" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E608" t="s">
         <v>15</v>
@@ -29562,7 +29562,7 @@
         <v>13</v>
       </c>
       <c r="D609" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E609" t="s">
         <v>15</v>
@@ -29603,7 +29603,7 @@
         <v>13</v>
       </c>
       <c r="D610" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E610" t="s">
         <v>15</v>
@@ -29644,7 +29644,7 @@
         <v>13</v>
       </c>
       <c r="D611" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E611" t="s">
         <v>15</v>

</xml_diff>